<commit_message>
added new intervention button
</commit_message>
<xml_diff>
--- a/tbs/templates/IMT_INT.xlsx
+++ b/tbs/templates/IMT_INT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\imt\production\tbs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\imt\tbs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2763C0-AC99-4477-90D7-6EADEFAEF9AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="R_A1" sheetId="1" r:id="rId1"/>
@@ -19,12 +18,12 @@
   <definedNames>
     <definedName name="the_named_cell">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>This sheet was hidden in the template, and it becomes visible.</t>
   </si>
@@ -116,9 +115,6 @@
     <t xml:space="preserve"> Internal Interventions</t>
   </si>
   <si>
-    <t>PAMANA Program</t>
-  </si>
-  <si>
     <t xml:space="preserve">Assistance to Individuals in Crisis Situations </t>
   </si>
   <si>
@@ -131,13 +127,70 @@
     <t>[a.col3;ope=tbs:num]</t>
   </si>
   <si>
-    <t>Other Interventions</t>
+    <t>Sustainable Livelihood Program (SLP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplementary Feeding Program (SFP) </t>
+  </si>
+  <si>
+    <t>Crisis Intervention (CIU)</t>
+  </si>
+  <si>
+    <t>Payapa at Masaganang Pamayanan (PAMANA)</t>
+  </si>
+  <si>
+    <t>Social Pension (SocPen)</t>
+  </si>
+  <si>
+    <t>Supplementary Feeding Program (SFP)</t>
+  </si>
+  <si>
+    <t>Protective Services Program</t>
+  </si>
+  <si>
+    <t>Community-Based Rehabilitation Program for Persons with Disabilities (CBR-PWD)</t>
+  </si>
+  <si>
+    <t>Recovery and Reintegration Program for Victims of Trafficking</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>[a.col4;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col5;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col6;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col7;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col8;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col9;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col10;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.col11;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.other;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -270,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -377,6 +430,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -421,73 +485,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -589,23 +653,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -641,23 +688,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -833,90 +863,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="8" width="16.5546875" customWidth="1"/>
-    <col min="12" max="13" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="8" width="16.5703125" customWidth="1"/>
+    <col min="12" max="13" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:23" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
     </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:23" s="5" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
     </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -933,7 +963,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="8"/>
       <c r="D6" s="6"/>
@@ -948,38 +978,38 @@
       <c r="M6" s="7"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:23" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="37" t="s">
+      <c r="J7" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="35" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="39" t="s">
@@ -987,46 +1017,91 @@
       </c>
       <c r="M7" s="40"/>
       <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="18" t="s">
+    <row r="8" spans="1:23" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="18" t="s">
+      <c r="N8" s="37" t="s">
         <v>35</v>
       </c>
+      <c r="O8" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="U8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="V8" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" s="37" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
+    <row r="9" spans="1:23" s="10" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>ROW()-9</f>
         <v>1</v>
@@ -1056,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>26</v>
@@ -1068,32 +1143,108 @@
         <v>25</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="V10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="W10" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="J11" s="14" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="15">
-        <f ca="1">SUM( K10                          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( K10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
       <c r="L11" s="15">
-        <f ca="1">SUM( L10                          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( L10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
       <c r="M11" s="15">
-        <f ca="1">SUM( M10                          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( M10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
       <c r="N11" s="15">
-        <f ca="1">SUM( N10                          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( N10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="15">
+        <f ca="1">SUM( O10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="15">
+        <f ca="1">SUM( P10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="15">
+        <f ca="1">SUM( Q10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
+        <f ca="1">SUM( R10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="15">
+        <f ca="1">SUM( S10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="15">
+        <f ca="1">SUM( T10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="15">
+        <f ca="1">SUM( U10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="15">
+        <f ca="1">SUM( V10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="15">
+        <f ca="1">SUM( W10                           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="28">
+    <mergeCell ref="L7:W7"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="W8:W9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
@@ -1106,13 +1257,9 @@
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L7:N7"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F7:F9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,7 +1268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -1129,14 +1276,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>

</xml_diff>